<commit_message>
fixed sticker based on context
</commit_message>
<xml_diff>
--- a/Stickers/0-sticker-to-number.xlsx
+++ b/Stickers/0-sticker-to-number.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Matteo\Coding\Discord_The_Archivist_Bot\Stickers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E5C959-F895-4580-B639-6D7147BCBA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3DCFBF-3DBE-4217-96D8-D7CC5E296FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4A16AD99-F915-4A35-A884-0E52F19CB173}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
   <si>
     <t>worms</t>
   </si>
@@ -302,6 +302,273 @@
   </si>
   <si>
     <t>sorry to love you and leave you but I gotta dash cheerio</t>
+  </si>
+  <si>
+    <t>Words</t>
+  </si>
+  <si>
+    <t>BRR</t>
+  </si>
+  <si>
+    <t>EGG</t>
+  </si>
+  <si>
+    <t>WORMS</t>
+  </si>
+  <si>
+    <t>LITERARY HEIGHTS</t>
+  </si>
+  <si>
+    <t>STATEMENT BEGINS</t>
+  </si>
+  <si>
+    <t>STATEMENT ENDS</t>
+  </si>
+  <si>
+    <t>DEFINE HURT</t>
+  </si>
+  <si>
+    <t>MICHEAL LAUGHTER</t>
+  </si>
+  <si>
+    <t>GERIATRIC CONSPIRACY</t>
+  </si>
+  <si>
+    <t>JONAH EVIL LAUGH</t>
+  </si>
+  <si>
+    <t>GOOD COWS</t>
+  </si>
+  <si>
+    <t>UNINSPIRED PERHAPS</t>
+  </si>
+  <si>
+    <t>SPOOKY GOOGLE</t>
+  </si>
+  <si>
+    <t>EVERYTHING</t>
+  </si>
+  <si>
+    <t>BADLY</t>
+  </si>
+  <si>
+    <t>DEAD IMPRESSED</t>
+  </si>
+  <si>
+    <t>TINGLY FEELING</t>
+  </si>
+  <si>
+    <t>BLANKET ANYTHING</t>
+  </si>
+  <si>
+    <t>SPIDER</t>
+  </si>
+  <si>
+    <t>SPIDERS FLIES</t>
+  </si>
+  <si>
+    <t>POLITE KNOCK</t>
+  </si>
+  <si>
+    <t>GHOST REALLY</t>
+  </si>
+  <si>
+    <t>TURNS SUGGESTION FIRE</t>
+  </si>
+  <si>
+    <t>BLANK BOOKS ALBERCHT</t>
+  </si>
+  <si>
+    <t>DEAD SERIOUS</t>
+  </si>
+  <si>
+    <t>PlACE NOW END</t>
+  </si>
+  <si>
+    <t>POWER ADMIT IMMUNE OCCASIONAL LAZY ASSUMPTION</t>
+  </si>
+  <si>
+    <t>EXPRESS DISAPPOINTMENT</t>
+  </si>
+  <si>
+    <t>HARD THINK</t>
+  </si>
+  <si>
+    <t>WORLD CREATED</t>
+  </si>
+  <si>
+    <t>BURN AMENABLE IDEA</t>
+  </si>
+  <si>
+    <t>FINEST CAT BURGLAR BROMLEY</t>
+  </si>
+  <si>
+    <t>SEEM LOT</t>
+  </si>
+  <si>
+    <t>SCREAMED ONCE</t>
+  </si>
+  <si>
+    <t>CERTAIN LO-FI CHARM</t>
+  </si>
+  <si>
+    <t>AM DEAL</t>
+  </si>
+  <si>
+    <t>BOOK APOCALYPSE</t>
+  </si>
+  <si>
+    <t>STONE COLD BITCH</t>
+  </si>
+  <si>
+    <t>RECORD SUBMISSION</t>
+  </si>
+  <si>
+    <t>PETTY RULES SPACE TIME</t>
+  </si>
+  <si>
+    <t>OVERSHADOWED</t>
+  </si>
+  <si>
+    <t>YOURSELF DOWN</t>
+  </si>
+  <si>
+    <t>FEELING FLAVOUR SEASONING</t>
+  </si>
+  <si>
+    <t>ANSWER MARTIN</t>
+  </si>
+  <si>
+    <t>TOUCHED</t>
+  </si>
+  <si>
+    <t>DINAMIC DUO</t>
+  </si>
+  <si>
+    <t>LOVE LEAVE DASH CHEERIO</t>
+  </si>
+  <si>
+    <t>OCCASIONALLY USEFUL</t>
+  </si>
+  <si>
+    <t>SHOCKER ESTEEM ISSUES POINT</t>
+  </si>
+  <si>
+    <t>EXPECT FACE</t>
+  </si>
+  <si>
+    <t>CHARACTER DROP PILOT</t>
+  </si>
+  <si>
+    <t>KILL BILL</t>
+  </si>
+  <si>
+    <t>MANIAC JOHNNY D'VILLE</t>
+  </si>
+  <si>
+    <t>RICH INNER LIFE</t>
+  </si>
+  <si>
+    <t>SOAP OPERA ARCHIVE</t>
+  </si>
+  <si>
+    <t>SLAP INTERRUPTS STATEMENT</t>
+  </si>
+  <si>
+    <t>DRUGS</t>
+  </si>
+  <si>
+    <t>TRAGIC ET CETERA</t>
+  </si>
+  <si>
+    <t>MEMENTO MORI</t>
+  </si>
+  <si>
+    <t>ATE SIMPLE</t>
+  </si>
+  <si>
+    <t>SCREAM</t>
+  </si>
+  <si>
+    <t>APOLOGIES DECEPTION</t>
+  </si>
+  <si>
+    <t>LISTENING</t>
+  </si>
+  <si>
+    <t>ADMITTEDLY POLISH LATIN</t>
+  </si>
+  <si>
+    <t>DEAD</t>
+  </si>
+  <si>
+    <t>UNFORGETTABLE</t>
+  </si>
+  <si>
+    <t>JIMMY MAGMA</t>
+  </si>
+  <si>
+    <t>BROADLY INTACT</t>
+  </si>
+  <si>
+    <t>JESUS REST</t>
+  </si>
+  <si>
+    <t>HATED WASTE ITALIANS</t>
+  </si>
+  <si>
+    <t>BIN</t>
+  </si>
+  <si>
+    <t>RATHER PERSONAL</t>
+  </si>
+  <si>
+    <t>LUCK DETECTIVE</t>
+  </si>
+  <si>
+    <t>TOMB LAUGHS</t>
+  </si>
+  <si>
+    <t>DOWN</t>
+  </si>
+  <si>
+    <t>MISUNDERSTANDING</t>
+  </si>
+  <si>
+    <t>HAND OWN STOMACH</t>
+  </si>
+  <si>
+    <t>CALLIOPE</t>
+  </si>
+  <si>
+    <t>DELICIOUS SCREAMING PASTA</t>
+  </si>
+  <si>
+    <t>BOO-OO MONSTER ALONE</t>
+  </si>
+  <si>
+    <t>SWANNING SAD</t>
+  </si>
+  <si>
+    <t>WINNING HUMOR</t>
+  </si>
+  <si>
+    <t>BRUTAL PEER REVIEW</t>
+  </si>
+  <si>
+    <t>RIB</t>
+  </si>
+  <si>
+    <t>INTENSELY BORING</t>
+  </si>
+  <si>
+    <t>feedback: less murder</t>
+  </si>
+  <si>
+    <t>FEEDBACK MURDER</t>
+  </si>
+  <si>
+    <t>LUCKY FALSE</t>
   </si>
 </sst>
 </file>
@@ -653,28 +920,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5893DE1A-31C9-4391-A0F6-ADF3F387E5F1}">
-  <dimension ref="A1:C89"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="90.5703125" customWidth="1"/>
-    <col min="3" max="3" width="95.7109375" customWidth="1"/>
+    <col min="3" max="3" width="78" customWidth="1"/>
+    <col min="4" max="4" width="52.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>42</v>
       </c>
       <c r="B1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -685,20 +956,26 @@
       <c r="C2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B89" si="0">UPPER(C3)</f>
+        <f t="shared" ref="B3:D89" si="0">UPPER(C3)</f>
         <v>WORMS</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -709,8 +986,11 @@
       <c r="C4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -721,8 +1001,11 @@
       <c r="C5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -733,8 +1016,11 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -745,8 +1031,11 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -757,8 +1046,11 @@
       <c r="C8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -769,8 +1061,11 @@
       <c r="C9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -782,7 +1077,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -793,8 +1088,11 @@
       <c r="C11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -805,8 +1103,11 @@
       <c r="C12" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -817,8 +1118,11 @@
       <c r="C13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -829,8 +1133,11 @@
       <c r="C14" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -841,8 +1148,11 @@
       <c r="C15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -853,8 +1163,11 @@
       <c r="C16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -865,8 +1178,11 @@
       <c r="C17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -877,8 +1193,11 @@
       <c r="C18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -889,8 +1208,11 @@
       <c r="C19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -901,8 +1223,11 @@
       <c r="C20" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -913,8 +1238,11 @@
       <c r="C21" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -925,8 +1253,11 @@
       <c r="C22" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -937,8 +1268,11 @@
       <c r="C23" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -949,8 +1283,11 @@
       <c r="C24" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -961,8 +1298,11 @@
       <c r="C25" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -973,8 +1313,11 @@
       <c r="C26" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -985,8 +1328,11 @@
       <c r="C27" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -997,8 +1343,11 @@
       <c r="C28" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1009,8 +1358,11 @@
       <c r="C29" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1021,8 +1373,11 @@
       <c r="C30" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1033,8 +1388,11 @@
       <c r="C31" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1045,8 +1403,11 @@
       <c r="C32" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1057,8 +1418,11 @@
       <c r="C33" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1069,8 +1433,11 @@
       <c r="C34" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1081,8 +1448,11 @@
       <c r="C35" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1093,8 +1463,11 @@
       <c r="C36" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1105,8 +1478,11 @@
       <c r="C37" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1117,8 +1493,11 @@
       <c r="C38" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1129,8 +1508,11 @@
       <c r="C39" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1141,8 +1523,11 @@
       <c r="C40" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1153,8 +1538,11 @@
       <c r="C41" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1165,8 +1553,11 @@
       <c r="C42" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1177,8 +1568,11 @@
       <c r="C43" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1189,8 +1583,11 @@
       <c r="C44" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1201,8 +1598,11 @@
       <c r="C45" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1213,8 +1613,11 @@
       <c r="C46" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1225,8 +1628,11 @@
       <c r="C47" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1237,8 +1643,11 @@
       <c r="C48" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1249,8 +1658,11 @@
       <c r="C49" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1261,8 +1673,11 @@
       <c r="C50" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1273,8 +1688,11 @@
       <c r="C51" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1285,8 +1703,11 @@
       <c r="C52" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1297,8 +1718,11 @@
       <c r="C53" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1309,8 +1733,11 @@
       <c r="C54" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1321,8 +1748,11 @@
       <c r="C55" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1333,8 +1763,11 @@
       <c r="C56" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1345,8 +1778,11 @@
       <c r="C57" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1357,8 +1793,11 @@
       <c r="C58" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1369,8 +1808,11 @@
       <c r="C59" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1381,8 +1823,11 @@
       <c r="C60" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1393,8 +1838,11 @@
       <c r="C61" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1405,8 +1853,11 @@
       <c r="C62" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1417,8 +1868,11 @@
       <c r="C63" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1429,8 +1883,11 @@
       <c r="C64" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1441,8 +1898,11 @@
       <c r="C65" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1453,8 +1913,11 @@
       <c r="C66" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1465,8 +1928,11 @@
       <c r="C67" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1477,8 +1943,11 @@
       <c r="C68" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1489,8 +1958,11 @@
       <c r="C69" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1501,8 +1973,11 @@
       <c r="C70" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1513,8 +1988,11 @@
       <c r="C71" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1525,8 +2003,11 @@
       <c r="C72" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1537,8 +2018,11 @@
       <c r="C73" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1549,8 +2033,11 @@
       <c r="C74" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1561,8 +2048,11 @@
       <c r="C75" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1573,8 +2063,11 @@
       <c r="C76" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -1585,8 +2078,11 @@
       <c r="C77" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -1597,8 +2093,11 @@
       <c r="C78" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -1609,8 +2108,11 @@
       <c r="C79" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -1621,8 +2123,11 @@
       <c r="C80" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -1633,8 +2138,11 @@
       <c r="C81" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -1645,8 +2153,11 @@
       <c r="C82" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -1657,8 +2168,11 @@
       <c r="C83" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -1669,8 +2183,11 @@
       <c r="C84" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -1681,8 +2198,11 @@
       <c r="C85" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -1693,20 +2213,26 @@
       <c r="C86" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87" t="str">
         <f t="shared" si="0"/>
-        <v>CALLIOPE</v>
+        <v>FEEDBACK: LESS MURDER</v>
       </c>
       <c r="C87" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="D87" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -1717,8 +2243,11 @@
       <c r="C88" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -1728,6 +2257,9 @@
       </c>
       <c r="C89" t="s">
         <v>68</v>
+      </c>
+      <c r="D89" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>